<commit_message>
ISP20220672 - [Final Ispection] 增加FGPT，相關程式依需求調整
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/FinalInspectionReport.xlsx
+++ b/Quality/Quality/XLT/FinalInspectionReport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Final Inspection Report</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -435,6 +435,10 @@
   </si>
   <si>
     <t xml:space="preserve">Color/ Shade: </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>FGPT:</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -685,7 +689,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -746,98 +750,101 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1141,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1154,17 +1161,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1176,109 +1183,109 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="34" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="40"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="36" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="41"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="36" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="36" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="41"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="36" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="41"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="36" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="41"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="38" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="46"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1291,558 +1298,538 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="21" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="39"/>
+      <c r="G13" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="26" t="s">
+      <c r="B17" s="42"/>
+      <c r="C17" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="21" t="s">
+      <c r="D17" s="42"/>
+      <c r="E17" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21" t="s">
+      <c r="F17" s="39"/>
+      <c r="G17" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21" t="s">
+      <c r="B19" s="39"/>
+      <c r="C19" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21" t="s">
+      <c r="D19" s="39"/>
+      <c r="E19" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21" t="s">
+      <c r="F19" s="39"/>
+      <c r="G19" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21" t="s">
+      <c r="B20" s="39"/>
+      <c r="C20" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21" t="s">
+      <c r="D20" s="39"/>
+      <c r="E20" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21" t="s">
+      <c r="F20" s="39"/>
+      <c r="G20" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21" t="s">
+      <c r="F22" s="39"/>
+      <c r="G22" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="29" t="s">
+      <c r="B24" s="49"/>
+      <c r="C24" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="5" t="s">
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="13"/>
-    </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="28"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="B27" s="46"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="42"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="5" t="s">
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="13"/>
-    </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="43"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="19" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="19" t="s">
+      <c r="D34" s="16"/>
+      <c r="E34" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B36" s="16"/>
       <c r="C36" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
+        <v>62</v>
+      </c>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="18"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="42" t="s">
+      <c r="D39" s="18"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="15"/>
-      <c r="C40" s="14" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="43" t="s">
+      <c r="D41" s="15"/>
+      <c r="E41" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="49"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="F41" s="30"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="33"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="14" t="s">
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F42" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G42" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14" t="s">
+      <c r="H42" s="14"/>
+      <c r="I42" s="14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-    </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="B45" s="35"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-    </row>
-    <row r="47" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B46" s="35"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+    </row>
+    <row r="48" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35" t="s">
-        <v>35</v>
-      </c>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="40"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="37" t="s">
-        <v>36</v>
-      </c>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="41"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B50" s="37"/>
+      <c r="B50" s="21"/>
       <c r="C50" s="37"/>
       <c r="D50" s="37"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="7"/>
+      <c r="E50" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="7"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B51" s="39"/>
-      <c r="C51" s="39"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="9"/>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="A39:I39"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
+  <mergeCells count="87">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="D37:I37"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="F32:I32"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
@@ -1853,27 +1840,61 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:I26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="D36:I36"/>
-    <mergeCell ref="D35:I35"/>
-    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A43:D43"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C46:I46"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ISP20231201 - Final Inspection Query功能調整
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/FinalInspectionReport.xlsx
+++ b/Quality/Quality/XLT/FinalInspectionReport.xlsx
@@ -11,12 +11,15 @@
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">工作表1!$A$1:$I$54</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Final Inspection Report</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -346,6 +349,10 @@
   </si>
   <si>
     <t>Carton Moisture Standard()</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signatrue</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -596,7 +603,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -615,18 +622,6 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -657,16 +652,76 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -681,55 +736,19 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1052,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:I40"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1065,17 +1084,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1087,109 +1106,109 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="34" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="36" t="s">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="41"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="36" t="s">
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="45"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="49"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="36" t="s">
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="41"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="36" t="s">
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="41"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="36" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="41"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="38" t="s">
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="46"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="50"/>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1202,10 +1221,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="33"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
@@ -1218,21 +1237,21 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
@@ -1245,32 +1264,32 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="29" t="s">
+      <c r="B18" s="36"/>
+      <c r="C18" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="31"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="13"/>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1278,43 +1297,43 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="21"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="13"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1322,82 +1341,82 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="17"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17" t="s">
+      <c r="B28" s="12"/>
+      <c r="C28" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="19" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="23"/>
@@ -1408,11 +1427,11 @@
       <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="17" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="13" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="23"/>
@@ -1423,7 +1442,7 @@
       <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="23"/>
@@ -1439,69 +1458,69 @@
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="18"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="14" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="43" t="s">
+      <c r="D35" s="11"/>
+      <c r="E35" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F35" s="43"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="49"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="53"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="14" t="s">
+      <c r="B36" s="47"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14" t="s">
+      <c r="H36" s="10"/>
+      <c r="I36" s="10" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
+      <c r="A37" s="46"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1510,30 +1529,41 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="50"/>
-      <c r="I39" s="50"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
     </row>
     <row r="42" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -1541,68 +1571,148 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35" t="s">
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="40"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="44"/>
-      <c r="D44" s="44"/>
-      <c r="E44" s="37" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="41"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="30"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="7"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="9"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+    </row>
+    <row r="48" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="24"/>
+      <c r="I50" s="24"/>
+    </row>
+    <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+    </row>
+    <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+    </row>
+    <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="74">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
+  <mergeCells count="86">
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="G52:I52"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G8:I8"/>
@@ -1614,38 +1724,28 @@
     <mergeCell ref="C40:I40"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:H19"/>
-    <mergeCell ref="F26:I26"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C16:D16"/>
@@ -1659,23 +1759,47 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:I43"/>
     <mergeCell ref="D30:I30"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="A50:C51"/>
+    <mergeCell ref="D50:F51"/>
+    <mergeCell ref="G50:I51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="A53:C54"/>
+    <mergeCell ref="D53:F54"/>
+    <mergeCell ref="G53:I54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
ISP20240684 - Privot 88格式調整
</commit_message>
<xml_diff>
--- a/Quality/Quality/XLT/FinalInspectionReport.xlsx
+++ b/Quality/Quality/XLT/FinalInspectionReport.xlsx
@@ -12,14 +12,14 @@
     <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">工作表1!$A$1:$I$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">工作表1!$A$1:$I$55</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>Final Inspection Report</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Brand:</t>
-  </si>
-  <si>
-    <t>Total SP# Qty:</t>
   </si>
   <si>
     <t>Inspection Stage:</t>
@@ -353,6 +350,14 @@
   </si>
   <si>
     <t>Signatrue</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Original PO#</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total SP# Qty:</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -673,39 +678,81 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -713,15 +760,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -734,39 +772,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1071,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:C51"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1084,17 +1089,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1106,14 +1111,14 @@
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="42" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
       <c r="D3" s="39"/>
-      <c r="E3" s="37" t="s">
-        <v>10</v>
+      <c r="E3" s="42" t="s">
+        <v>9</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="38"/>
@@ -1128,7 +1133,7 @@
       <c r="C4" s="28"/>
       <c r="D4" s="30"/>
       <c r="E4" s="27" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
@@ -1143,12 +1148,12 @@
       <c r="C5" s="28"/>
       <c r="D5" s="30"/>
       <c r="E5" s="27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="49"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
@@ -1158,12 +1163,12 @@
       <c r="C6" s="28"/>
       <c r="D6" s="30"/>
       <c r="E6" s="27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="30"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="27" t="s">
@@ -1173,7 +1178,7 @@
       <c r="C7" s="28"/>
       <c r="D7" s="30"/>
       <c r="E7" s="27" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
@@ -1188,7 +1193,7 @@
       <c r="C8" s="28"/>
       <c r="D8" s="30"/>
       <c r="E8" s="27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
@@ -1196,606 +1201,623 @@
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="25" t="s">
+      <c r="A9" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="50"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="45"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="48" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="46"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="49"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="52"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="37" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="44" t="s">
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
+        <v>40</v>
+      </c>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="11"/>
+      <c r="E36" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F36" s="32"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="34"/>
+      <c r="I36" s="35"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="14"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46"/>
-      <c r="I34" s="46"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="53"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="46"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="36"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="54"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="54"/>
-      <c r="I39" s="54"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
+      <c r="B41" s="37"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+    </row>
+    <row r="43" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="44"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="46"/>
-      <c r="I40" s="46"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-    </row>
-    <row r="42" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="39"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="28"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="30"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="39"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B45" s="28"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="28"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="28"/>
+      <c r="I45" s="30"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="18"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="18"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-    </row>
-    <row r="48" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="23"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="23"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+    </row>
+    <row r="49" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="26"/>
+      <c r="I50" s="26"/>
     </row>
     <row r="51" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-    </row>
-    <row r="52" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="23"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="23"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="25"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
     </row>
     <row r="54" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
+  <mergeCells count="90">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G51:I52"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="A54:C55"/>
+    <mergeCell ref="D54:F55"/>
+    <mergeCell ref="G54:I55"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="A51:C52"/>
+    <mergeCell ref="D51:F52"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="F29:I29"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A35:I35"/>
     <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="D31:I31"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:H19"/>
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:H20"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="D30:I30"/>
-    <mergeCell ref="F28:I28"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A25:I25"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="A50:C51"/>
-    <mergeCell ref="D50:F51"/>
-    <mergeCell ref="G50:I51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="A53:C54"/>
-    <mergeCell ref="D53:F54"/>
-    <mergeCell ref="G53:I54"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="D32:I32"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A28:I28"/>
+    <mergeCell ref="A30:I30"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>